<commit_message>
Adding New Test Suites
</commit_message>
<xml_diff>
--- a/testScripts/TestData.xlsx
+++ b/testScripts/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>Response</t>
   </si>
@@ -124,6 +124,24 @@
     <t>HTTP/1.1 200 
 Content-Type: application/java; charset=UTF-8
 Date: Mon, 01 Jul 2019 13:10:05 GMT
+Server: nginx
+Content-Length: 13
+Connection: keep-alive
+CI/CD Demo...</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 
+Content-Type: application/java; charset=UTF-8
+Date: Tue, 02 Jul 2019 01:25:26 GMT
+Server: nginx
+Content-Length: 13
+Connection: keep-alive
+CI/CD Demo...</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 200 
+Content-Type: application/java; charset=UTF-8
+Date: Tue, 02 Jul 2019 01:25:28 GMT
 Server: nginx
 Content-Length: 13
 Connection: keep-alive
@@ -503,10 +521,10 @@
     </row>
     <row r="2" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>400</v>
@@ -514,7 +532,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -525,7 +543,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>